<commit_message>
Update Tugas Prioritas 1
</commit_message>
<xml_diff>
--- a/4_Testing Document (Test Scenario-Test Case-dll)/Praktikum/Sec 4 - Test Documentation - Soal Prioritas 1.xlsx
+++ b/4_Testing Document (Test Scenario-Test Case-dll)/Praktikum/Sec 4 - Test Documentation - Soal Prioritas 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\MSIB\Batch 4\Alterra- SQE\Task\Task Sec 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\MSIB\Batch 4\Alterra- SQE\Task\Task Sec 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B0FE8A-925C-4BED-80E4-8B8528E7B674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37CD80A-DEB1-47BF-B86E-CA52E005A1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{188708C7-0C4D-40BD-B380-A54F6206D690}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{188708C7-0C4D-40BD-B380-A54F6206D690}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -217,9 +217,6 @@
     <t>Login failed if email is valid and password is invalid</t>
   </si>
   <si>
-    <t>Login failed if email is valid and password is valid</t>
-  </si>
-  <si>
     <t>1. Input an invalid phone number
 2. Input an valid password
 3. Click the "Login" button</t>
@@ -477,6 +474,9 @@
   </si>
   <si>
     <t>Phone number: 0859568****</t>
+  </si>
+  <si>
+    <t>Login failed if email is invalid and password is invalid</t>
   </si>
 </sst>
 </file>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA99C2B-47B1-4F90-83FA-3D5537CE2417}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1070,7 @@
         <v>19</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1090,7 +1090,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>47</v>
@@ -1111,7 +1111,7 @@
         <v>26</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1131,7 +1131,7 @@
         <v>43</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>48</v>
@@ -1152,7 +1152,7 @@
         <v>26</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1172,7 +1172,7 @@
         <v>43</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>49</v>
@@ -1193,7 +1193,7 @@
         <v>26</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1204,7 +1204,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>51</v>
@@ -1213,7 +1213,7 @@
         <v>43</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>50</v>
@@ -1234,7 +1234,7 @@
         <v>26</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>52</v>
@@ -1254,7 +1254,7 @@
         <v>22</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>53</v>
@@ -1275,7 +1275,7 @@
         <v>26</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1286,7 +1286,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>52</v>
@@ -1295,10 +1295,10 @@
         <v>43</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>44</v>
@@ -1316,7 +1316,7 @@
         <v>26</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1327,7 +1327,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>52</v>
@@ -1336,7 +1336,7 @@
         <v>43</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>53</v>
@@ -1357,7 +1357,7 @@
         <v>26</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1368,7 +1368,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>52</v>
@@ -1377,7 +1377,7 @@
         <v>43</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>48</v>
@@ -1398,7 +1398,7 @@
         <v>26</v>
       </c>
       <c r="M17" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1406,28 +1406,28 @@
         <v>34</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J18" s="12">
         <v>44980</v>
@@ -1439,7 +1439,7 @@
         <v>26</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1447,28 +1447,28 @@
         <v>35</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>43</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="12">
         <v>44980</v>
@@ -1480,7 +1480,7 @@
         <v>26</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1488,28 +1488,28 @@
         <v>36</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>85</v>
-      </c>
       <c r="D20" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J20" s="12">
         <v>44980</v>
@@ -1521,7 +1521,7 @@
         <v>26</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1529,28 +1529,28 @@
         <v>37</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>43</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G21" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="H21" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="I21" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J21" s="12">
         <v>44980</v>
@@ -1562,7 +1562,7 @@
         <v>26</v>
       </c>
       <c r="M21" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -1570,28 +1570,28 @@
         <v>38</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J22" s="12">
         <v>44980</v>
@@ -1603,7 +1603,7 @@
         <v>26</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -1611,28 +1611,28 @@
         <v>39</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J23" s="12">
         <v>44980</v>
@@ -1644,7 +1644,7 @@
         <v>26</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -1652,28 +1652,28 @@
         <v>40</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J24" s="12">
         <v>44980</v>
@@ -1685,7 +1685,7 @@
         <v>26</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1693,28 +1693,28 @@
         <v>41</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F25" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G25" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="H25" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J25" s="12">
         <v>44980</v>
@@ -1726,7 +1726,7 @@
         <v>26</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1734,28 +1734,28 @@
         <v>42</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>43</v>
       </c>
       <c r="F26" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G26" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="H26" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J26" s="12">
         <v>44980</v>
@@ -1767,7 +1767,7 @@
         <v>26</v>
       </c>
       <c r="M26" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>